<commit_message>
Checking create DB and conexion
He realizado la conexion entre la base de datos y nuestro IDE
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -735,20 +735,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="47.77734375" customWidth="1"/>
-    <col min="2" max="2" width="29.21875" customWidth="1"/>
-    <col min="3" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="61.21875" customWidth="1"/>
-    <col min="7" max="7" width="29.21875" customWidth="1"/>
+    <col min="1" max="1" width="47.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="61.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +786,7 @@
       <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
         <v>7</v>
@@ -805,7 +805,7 @@
       <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="3"/>
       <c r="F4" s="6" t="s">
         <v>4</v>
@@ -981,7 +981,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="17.399999999999999">
+    <row r="14" spans="1:7" ht="18">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="17.399999999999999">
+    <row r="19" spans="1:7" ht="18">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="17.399999999999999">
+    <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="17.399999999999999">
+    <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Checking permissions DB and use od JDBC
Hemos realizado los permisos, la creacion de las tablas serie y plataforma y el uso de JDBC
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -736,7 +736,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -919,7 +919,7 @@
       <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="3"/>
       <c r="F10" s="6" t="s">
         <v>19</v>
@@ -1157,7 +1157,7 @@
       <c r="C26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>

</xml_diff>

<commit_message>
Checking some options of classes an update files on github
He realizado algunas cosas mas de prioridad alta
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -736,7 +736,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -881,7 +881,7 @@
       <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="3"/>
       <c r="F8" s="6" t="s">
         <v>14</v>
@@ -1025,7 +1025,7 @@
       <c r="C16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1082,7 +1082,7 @@
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>

</xml_diff>

<commit_message>
Checking of the List
Hemos realizado varios requisitos del trabajo
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -735,20 +735,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="61.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="61.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:7" ht="17.399999999999999">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
         <v>9</v>
@@ -843,7 +843,7 @@
       <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="3"/>
       <c r="F6" s="6" t="s">
         <v>11</v>
@@ -862,7 +862,7 @@
       <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
         <v>13</v>
@@ -976,12 +976,12 @@
       <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="18">
+    <row r="14" spans="1:7" ht="17.399999999999999">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1048,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" ht="18">
+    <row r="19" spans="1:7" ht="17.399999999999999">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1127,7 +1127,7 @@
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1172,7 +1172,7 @@
       <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1240,7 +1240,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="18">
+    <row r="33" spans="1:7" ht="17.399999999999999">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="18">
+    <row r="34" spans="1:7" ht="17.399999999999999">
       <c r="A34" s="2" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Upload of UML and some checkings
He generado el UML del trabajo de Java y he realizado el proyecto autonomo y la organizacion de codigo
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>RF1</t>
   </si>
@@ -184,13 +184,16 @@
   </si>
   <si>
     <t>REQUISITOS A REALIZAR SEGUNDA SEMANA</t>
+  </si>
+  <si>
+    <t>UML GENERADO EN NETBEANS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -279,6 +282,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Liberation Sans"/>
     </font>
   </fonts>
@@ -453,7 +461,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,6 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="2"/>
@@ -539,6 +548,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>686371</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>38633</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="6193971"/>
+          <a:ext cx="17200000" cy="8181148"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -804,15 +856,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:G21"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="61.33203125" customWidth="1"/>
@@ -1022,7 +1074,7 @@
       <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8" t="s">
         <v>22</v>
@@ -1164,7 +1216,7 @@
       <c r="G19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="13.35" customHeight="1">
       <c r="A20" s="11"/>
@@ -1198,7 +1250,7 @@
       <c r="G21" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="15"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="6" t="s">
@@ -1230,7 +1282,7 @@
       <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="23"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="3"/>
       <c r="F23" s="19" t="s">
         <v>28</v>
@@ -1404,6 +1456,11 @@
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
     </row>
+    <row r="37" spans="1:8" ht="22.8">
+      <c r="A37" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1411,5 +1468,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Checking entrega en carpeta compartida
Ya he realizado la entrega del proyecto a Dario
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -1230,7 +1230,7 @@
       <c r="G20" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="4" t="s">
@@ -1370,7 +1370,7 @@
       <c r="C28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="23"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="3"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>

</xml_diff>

<commit_message>
Checking of the Last Requirements
Damos el proyecto por finalizado al marcar todas las opciones de la lista de requisitos fundamentales y no fundamentales
</commit_message>
<xml_diff>
--- a/Entornos.xlsx
+++ b/Entornos.xlsx
@@ -293,7 +293,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +388,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -464,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -508,12 +502,11 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -900,7 +893,7 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -1135,7 +1128,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="3"/>
       <c r="F12" s="6" t="s">
         <v>25</v>
@@ -1193,7 +1186,7 @@
       <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="3"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1285,10 +1278,10 @@
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="25" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="16"/>
@@ -1311,7 +1304,7 @@
       <c r="G22" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
@@ -1351,7 +1344,7 @@
       <c r="G24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="4" t="s">
@@ -1366,7 +1359,7 @@
       <c r="D25" s="13"/>
       <c r="E25" s="3"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8">
@@ -1498,12 +1491,12 @@
       <c r="H34" s="15"/>
     </row>
     <row r="37" spans="1:8" ht="22.8">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="22.8">
-      <c r="A89" s="27" t="s">
+      <c r="A89" s="26" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>